<commit_message>
load data for subject
</commit_message>
<xml_diff>
--- a/room.xlsx
+++ b/room.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
-  <si>
-    <t xml:space="preserve">mã phòng </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t xml:space="preserve">Tên phòng </t>
   </si>
@@ -70,7 +67,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +86,12 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -209,7 +212,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -222,31 +225,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -270,6 +270,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1366,9 +1367,7 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
@@ -1389,24 +1388,20 @@
     </row>
     <row r="2" ht="14.55" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4"/>
+      <c r="C2" t="s" s="5">
         <v>0</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="D2" t="s" s="5">
         <v>1</v>
-      </c>
-      <c r="D2" t="s" s="5">
-        <v>2</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" ht="14.35" customHeight="1">
       <c r="A3" s="7"/>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
+      <c r="B3" s="8"/>
       <c r="C3" t="s" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="10">
         <v>30</v>
@@ -1415,11 +1410,9 @@
     </row>
     <row r="4" ht="14.35" customHeight="1">
       <c r="A4" s="7"/>
-      <c r="B4" s="8">
-        <v>2</v>
-      </c>
+      <c r="B4" s="8"/>
       <c r="C4" t="s" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="10">
         <v>30</v>
@@ -1428,11 +1421,9 @@
     </row>
     <row r="5" ht="14.35" customHeight="1">
       <c r="A5" s="7"/>
-      <c r="B5" s="8">
-        <v>3</v>
-      </c>
+      <c r="B5" s="8"/>
       <c r="C5" t="s" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="10">
         <v>35</v>
@@ -1441,11 +1432,9 @@
     </row>
     <row r="6" ht="14.35" customHeight="1">
       <c r="A6" s="7"/>
-      <c r="B6" s="8">
-        <v>4</v>
-      </c>
+      <c r="B6" s="8"/>
       <c r="C6" t="s" s="9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="10">
         <v>35</v>
@@ -1454,11 +1443,9 @@
     </row>
     <row r="7" ht="14.35" customHeight="1">
       <c r="A7" s="7"/>
-      <c r="B7" s="8">
-        <v>5</v>
-      </c>
+      <c r="B7" s="8"/>
       <c r="C7" t="s" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="10">
         <v>40</v>
@@ -1467,11 +1454,9 @@
     </row>
     <row r="8" ht="14.35" customHeight="1">
       <c r="A8" s="7"/>
-      <c r="B8" s="8">
-        <v>6</v>
-      </c>
+      <c r="B8" s="8"/>
       <c r="C8" t="s" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="10">
         <v>20</v>
@@ -1480,11 +1465,9 @@
     </row>
     <row r="9" ht="14.35" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="8">
-        <v>7</v>
-      </c>
+      <c r="B9" s="8"/>
       <c r="C9" t="s" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="10">
         <v>20</v>
@@ -1493,11 +1476,9 @@
     </row>
     <row r="10" ht="14.35" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="8">
-        <v>8</v>
-      </c>
+      <c r="B10" s="8"/>
       <c r="C10" t="s" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="10">
         <v>40</v>
@@ -1506,70 +1487,70 @@
     </row>
     <row r="11" ht="14.35" customHeight="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="12"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
     </row>
     <row r="12" ht="14.35" customHeight="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="12"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
     </row>
     <row r="13" ht="14.35" customHeight="1">
       <c r="A13" s="7"/>
-      <c r="B13" s="12"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
     <row r="14" ht="14.35" customHeight="1">
       <c r="A14" s="7"/>
-      <c r="B14" s="12"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
     </row>
     <row r="15" ht="14.35" customHeight="1">
       <c r="A15" s="7"/>
-      <c r="B15" s="12"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
     </row>
     <row r="16" ht="14.35" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="12"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
     </row>
     <row r="17" ht="14.35" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="12"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
     </row>
     <row r="18" ht="14.35" customHeight="1">
       <c r="A18" s="7"/>
-      <c r="B18" s="12"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
     </row>
     <row r="19" ht="14.35" customHeight="1">
       <c r="A19" s="7"/>
-      <c r="B19" s="12"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
     </row>
     <row r="20" ht="14.35" customHeight="1">
       <c r="A20" s="7"/>
-      <c r="B20" s="12"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>

</xml_diff>